<commit_message>
add temp info page, excel change
</commit_message>
<xml_diff>
--- a/test/xlsx/example.xlsx
+++ b/test/xlsx/example.xlsx
@@ -22,16 +22,17 @@
     <t>Фото ГРЗ</t>
   </si>
   <si>
-    <t>Камера</t>
-  </si>
-  <si>
-    <t>Дата и время события</t>
-  </si>
-  <si>
-    <t>Распознанный номер</t>
-  </si>
-  <si>
-    <t>Марка</t>
+    <t>ID Камеры</t>
+  </si>
+  <si>
+    <t>Дата и время события 
+ гггг.мм.дд чч:мм:сс</t>
+  </si>
+  <si>
+    <t>Распознанный ГРЗ</t>
+  </si>
+  <si>
+    <t>Тип авто</t>
   </si>
   <si>
     <t>TCENT_NAO_131_68_1; ТЦ МЕГА Теплый Стан. Калужский мост-въезд\r\n#ГРЗ (номера)</t>
@@ -90,15 +91,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF396CB4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,14 +113,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -154,7 +179,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="190500"/>
+          <a:off x="0" y="504825"/>
           <a:ext cx="2133600" cy="2133600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -192,7 +217,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2305050" y="381000"/>
+          <a:off x="2305050" y="695325"/>
           <a:ext cx="1914525" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -230,7 +255,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2343150"/>
+          <a:off x="0" y="2657475"/>
           <a:ext cx="2133600" cy="2133600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -268,7 +293,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2305050" y="2533650"/>
+          <a:off x="2305050" y="2847975"/>
           <a:ext cx="1914525" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -306,7 +331,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4495800"/>
+          <a:off x="0" y="4810125"/>
           <a:ext cx="2133600" cy="2133600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -344,7 +369,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2305050" y="4686300"/>
+          <a:off x="2305050" y="5000625"/>
           <a:ext cx="1914525" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -382,7 +407,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6648450"/>
+          <a:off x="0" y="6962775"/>
           <a:ext cx="2133600" cy="2133600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -420,7 +445,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2305050" y="6838950"/>
+          <a:off x="2305050" y="7153275"/>
           <a:ext cx="1914525" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -724,26 +749,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="31.7109375" style="1" customWidth="1"/>
+    <col min="1" max="6" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="40" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>